<commit_message>
removed junk and updated siteurl
</commit_message>
<xml_diff>
--- a/bin/com/uat/xls/TM_Project_Suite.xlsx
+++ b/bin/com/uat/xls/TM_Project_Suite.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="80">
   <si>
     <t>TCID</t>
   </si>
@@ -323,9 +323,6 @@
     <t>Verify Start End Date</t>
   </si>
   <si>
-    <t>24/03/2017</t>
-  </si>
-  <si>
     <t>1/6/2017</t>
   </si>
   <si>
@@ -335,23 +332,19 @@
     <t>VerifyStartEndDateValidation</t>
   </si>
   <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>End Dat should always be greater or equal to the Start Dat!</t>
-  </si>
-  <si>
-    <t>Test User</t>
-  </si>
-  <si>
-    <t>expected [End Dat should always be greater or equal to the Start Dat!] but found []</t>
+    <t>End Date should always be greater or equal to the Start Date!</t>
+  </si>
+  <si>
+    <t>24/04/2017</t>
+  </si>
+  <si>
+    <t>test demo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -848,18 +841,18 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="40.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="38.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="80.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="94.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.3984375" collapsed="true"/>
+    <col min="1" max="1" width="40.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="38.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="80" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="94.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -884,19 +877,17 @@
     </row>
     <row r="2" spans="1:6" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>76</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>77</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
       <c r="E2" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>78</v>
-      </c>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -986,10 +977,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="1" max="1" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1066,8 +1057,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="80.85546875" collapsed="true"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="80.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1113,9 +1104,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1191,26 +1182,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="49.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="46.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="47.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="9.140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="17" max="18" customWidth="true" width="31.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="44.85546875" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="35.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="255.0" collapsed="true"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="46.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="47.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="8.7109375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="20" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="17" max="18" width="31.7109375" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="44.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="35.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="255" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
@@ -1371,22 +1362,22 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="49.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="46.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="47.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="35.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="6.3984375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="74.96484375" collapsed="true"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="46.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="47.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="35.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -1444,26 +1435,21 @@
         <v>53</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J2" t="s">
         <v>51</v>
       </c>
-      <c r="K2" t="s">
-        <v>78</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="L2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>